<commit_message>
the very first step
</commit_message>
<xml_diff>
--- a/studentInput1.xlsx
+++ b/studentInput1.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26230"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nodejs\setup\workspace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/STUDY/大三下/软件工程/Sunshine-Interview-Server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBF810D-AFB9-4169-A169-9D879883C565}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9797CDDD-DD6C-4321-8722-24050809753D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="91">
   <si>
     <t>博雅楼101教室</t>
   </si>
@@ -277,12 +279,61 @@
   </si>
   <si>
     <t>4643880864@qq.cn</t>
+  </si>
+  <si>
+    <t>地点</t>
+    <rPh sb="0" eb="1">
+      <t>di dian</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始时间</t>
+    <rPh sb="0" eb="1">
+      <t>kai shi shi j</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结束时间</t>
+    <rPh sb="0" eb="1">
+      <t>jie shu shi j</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>准考证号</t>
+    <rPh sb="0" eb="1">
+      <t>zhun kao zheng hao</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名</t>
+    <rPh sb="0" eb="1">
+      <t>xing m</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮箱</t>
+    <rPh sb="0" eb="1">
+      <t>you xiang</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电话</t>
+    <rPh sb="0" eb="1">
+      <t>dian hua</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -645,39 +696,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3E8A83-CCF9-4829-922D-A6A1F5CD6AA6}">
-  <dimension ref="A1:G40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="25" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="25" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2">
-        <v>43628.583333333336</v>
-      </c>
-      <c r="C1" s="2">
-        <v>43627.618055555555</v>
-      </c>
-      <c r="D1" s="1">
-        <v>12000000</v>
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1">
-        <v>13764517513</v>
+        <v>89</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -691,16 +742,16 @@
         <v>43627.618055555555</v>
       </c>
       <c r="D2" s="1">
-        <v>12000004</v>
+        <v>12000000</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1">
-        <v>18497330870</v>
+        <v>13764517513</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -714,16 +765,16 @@
         <v>43627.618055555555</v>
       </c>
       <c r="D3" s="1">
-        <v>12000008</v>
+        <v>12000004</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G3" s="1">
-        <v>18507601276</v>
+        <v>18497330870</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -737,16 +788,16 @@
         <v>43627.618055555555</v>
       </c>
       <c r="D4" s="1">
-        <v>12000012</v>
+        <v>12000008</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G4" s="1">
-        <v>18343365979</v>
+        <v>18507601276</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -760,16 +811,16 @@
         <v>43627.618055555555</v>
       </c>
       <c r="D5" s="1">
-        <v>12000016</v>
+        <v>12000012</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G5" s="1">
-        <v>18431633933</v>
+        <v>18343365979</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -777,22 +828,22 @@
         <v>0</v>
       </c>
       <c r="B6" s="2">
-        <v>43628.625</v>
+        <v>43628.583333333336</v>
       </c>
       <c r="C6" s="2">
-        <v>43627.659722222219</v>
+        <v>43627.618055555555</v>
       </c>
       <c r="D6" s="1">
-        <v>12000009</v>
+        <v>12000016</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1">
-        <v>13788663652</v>
+        <v>18431633933</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -806,16 +857,16 @@
         <v>43627.659722222219</v>
       </c>
       <c r="D7" s="1">
-        <v>12000013</v>
+        <v>12000009</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1">
-        <v>18528991903</v>
+        <v>13788663652</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -829,16 +880,16 @@
         <v>43627.659722222219</v>
       </c>
       <c r="D8" s="1">
-        <v>12000017</v>
+        <v>12000013</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G8" s="1">
-        <v>18949523666</v>
+        <v>18528991903</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -852,16 +903,16 @@
         <v>43627.659722222219</v>
       </c>
       <c r="D9" s="1">
-        <v>12000001</v>
+        <v>12000017</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G9" s="1">
-        <v>18480244071</v>
+        <v>18949523666</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -875,39 +926,39 @@
         <v>43627.659722222219</v>
       </c>
       <c r="D10" s="1">
-        <v>12000005</v>
+        <v>12000001</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G10" s="1">
-        <v>18879790991</v>
+        <v>18480244071</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B11" s="2">
-        <v>43628.583333333336</v>
+        <v>43628.625</v>
       </c>
       <c r="C11" s="2">
-        <v>43627.618055555555</v>
+        <v>43627.659722222219</v>
       </c>
       <c r="D11" s="1">
-        <v>12000002</v>
+        <v>12000005</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G11" s="1">
-        <v>13511311080</v>
+        <v>18879790991</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -921,16 +972,16 @@
         <v>43627.618055555555</v>
       </c>
       <c r="D12" s="1">
-        <v>12000006</v>
+        <v>12000002</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G12" s="1">
-        <v>13696350422</v>
+        <v>13511311080</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -944,16 +995,16 @@
         <v>43627.618055555555</v>
       </c>
       <c r="D13" s="1">
-        <v>12000010</v>
+        <v>12000006</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G13" s="1">
-        <v>13674423549</v>
+        <v>13696350422</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -967,16 +1018,16 @@
         <v>43627.618055555555</v>
       </c>
       <c r="D14" s="1">
-        <v>12000014</v>
+        <v>12000010</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G14" s="1">
-        <v>18610270181</v>
+        <v>13674423549</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -990,16 +1041,16 @@
         <v>43627.618055555555</v>
       </c>
       <c r="D15" s="1">
-        <v>12000018</v>
+        <v>12000014</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G15" s="1">
-        <v>18400340568</v>
+        <v>18610270181</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1007,22 +1058,22 @@
         <v>21</v>
       </c>
       <c r="B16" s="2">
-        <v>43628.625</v>
+        <v>43628.583333333336</v>
       </c>
       <c r="C16" s="2">
-        <v>43627.659722222219</v>
+        <v>43627.618055555555</v>
       </c>
       <c r="D16" s="1">
-        <v>12000003</v>
+        <v>12000018</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G16" s="1">
-        <v>13351380403</v>
+        <v>18400340568</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1036,16 +1087,16 @@
         <v>43627.659722222219</v>
       </c>
       <c r="D17" s="1">
-        <v>12000007</v>
+        <v>12000003</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G17" s="1">
-        <v>13589254211</v>
+        <v>13351380403</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1059,16 +1110,16 @@
         <v>43627.659722222219</v>
       </c>
       <c r="D18" s="1">
-        <v>12000011</v>
+        <v>12000007</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G18" s="1">
-        <v>13881483647</v>
+        <v>13589254211</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1082,16 +1133,16 @@
         <v>43627.659722222219</v>
       </c>
       <c r="D19" s="1">
-        <v>12000015</v>
+        <v>12000011</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G19" s="1">
-        <v>13867485315</v>
+        <v>13881483647</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1105,39 +1156,39 @@
         <v>43627.659722222219</v>
       </c>
       <c r="D20" s="1">
-        <v>12000019</v>
+        <v>12000015</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G20" s="1">
-        <v>18898251628</v>
+        <v>13867485315</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>43627.375</v>
+        <v>43628.625</v>
       </c>
       <c r="C21" s="2">
-        <v>43627.409722222219</v>
+        <v>43627.659722222219</v>
       </c>
       <c r="D21" s="1">
-        <v>11000006</v>
+        <v>12000019</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G21" s="1">
-        <v>18701027128</v>
+        <v>18898251628</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1151,16 +1202,16 @@
         <v>43627.409722222219</v>
       </c>
       <c r="D22" s="1">
-        <v>11000010</v>
+        <v>11000006</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G22" s="1">
-        <v>18702634284</v>
+        <v>18701027128</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1174,16 +1225,16 @@
         <v>43627.409722222219</v>
       </c>
       <c r="D23" s="1">
-        <v>11000014</v>
+        <v>11000010</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G23" s="1">
-        <v>13711852218</v>
+        <v>18702634284</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1197,16 +1248,16 @@
         <v>43627.409722222219</v>
       </c>
       <c r="D24" s="1">
-        <v>11000018</v>
+        <v>11000014</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G24" s="1">
-        <v>13917028903</v>
+        <v>13711852218</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1220,16 +1271,16 @@
         <v>43627.409722222219</v>
       </c>
       <c r="D25" s="1">
-        <v>11000002</v>
+        <v>11000018</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G25" s="1">
-        <v>18892748534</v>
+        <v>13917028903</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1237,22 +1288,22 @@
         <v>42</v>
       </c>
       <c r="B26" s="2">
-        <v>43627.416666666664</v>
+        <v>43627.375</v>
       </c>
       <c r="C26" s="2">
-        <v>43627.451388888891</v>
+        <v>43627.409722222219</v>
       </c>
       <c r="D26" s="1">
-        <v>11000019</v>
+        <v>11000002</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G26" s="1">
-        <v>13412384996</v>
+        <v>18892748534</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1266,16 +1317,16 @@
         <v>43627.451388888891</v>
       </c>
       <c r="D27" s="1">
-        <v>11000003</v>
+        <v>11000019</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G27" s="1">
-        <v>18651954818</v>
+        <v>13412384996</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1289,16 +1340,16 @@
         <v>43627.451388888891</v>
       </c>
       <c r="D28" s="1">
-        <v>11000007</v>
+        <v>11000003</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G28" s="1">
-        <v>13453916075</v>
+        <v>18651954818</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1312,16 +1363,16 @@
         <v>43627.451388888891</v>
       </c>
       <c r="D29" s="1">
-        <v>11000011</v>
+        <v>11000007</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G29" s="1">
-        <v>13480258914</v>
+        <v>13453916075</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1335,39 +1386,39 @@
         <v>43627.451388888891</v>
       </c>
       <c r="D30" s="1">
-        <v>11000015</v>
+        <v>11000011</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G30" s="1">
-        <v>18495570983</v>
+        <v>13480258914</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B31" s="2">
-        <v>43627.375</v>
+        <v>43627.416666666664</v>
       </c>
       <c r="C31" s="2">
-        <v>43627.409722222219</v>
+        <v>43627.451388888891</v>
       </c>
       <c r="D31" s="1">
-        <v>11000012</v>
+        <v>11000015</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G31" s="1">
-        <v>13413054593</v>
+        <v>18495570983</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1381,16 +1432,16 @@
         <v>43627.409722222219</v>
       </c>
       <c r="D32" s="1">
-        <v>11000016</v>
+        <v>11000012</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G32" s="1">
-        <v>13389820840</v>
+        <v>13413054593</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1404,16 +1455,16 @@
         <v>43627.409722222219</v>
       </c>
       <c r="D33" s="1">
-        <v>11000000</v>
+        <v>11000016</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G33" s="1">
-        <v>18327519127</v>
+        <v>13389820840</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1427,16 +1478,16 @@
         <v>43627.409722222219</v>
       </c>
       <c r="D34" s="1">
-        <v>11000004</v>
+        <v>11000000</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G34" s="1">
-        <v>13754572439</v>
+        <v>18327519127</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1450,16 +1501,16 @@
         <v>43627.409722222219</v>
       </c>
       <c r="D35" s="1">
-        <v>11000008</v>
+        <v>11000004</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G35" s="1">
-        <v>18783245155</v>
+        <v>13754572439</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1467,22 +1518,22 @@
         <v>63</v>
       </c>
       <c r="B36" s="2">
-        <v>43627.416666666664</v>
+        <v>43627.375</v>
       </c>
       <c r="C36" s="2">
-        <v>43627.451388888891</v>
+        <v>43627.409722222219</v>
       </c>
       <c r="D36" s="1">
-        <v>11000001</v>
+        <v>11000008</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G36" s="1">
-        <v>18683179950</v>
+        <v>18783245155</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1496,16 +1547,16 @@
         <v>43627.451388888891</v>
       </c>
       <c r="D37" s="1">
-        <v>11000005</v>
+        <v>11000001</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G37" s="1">
-        <v>13779837466</v>
+        <v>18683179950</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1519,16 +1570,16 @@
         <v>43627.451388888891</v>
       </c>
       <c r="D38" s="1">
-        <v>11000009</v>
+        <v>11000005</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G38" s="1">
-        <v>13692528790</v>
+        <v>13779837466</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1542,16 +1593,16 @@
         <v>43627.451388888891</v>
       </c>
       <c r="D39" s="1">
-        <v>11000013</v>
+        <v>11000009</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G39" s="1">
-        <v>13954859886</v>
+        <v>13692528790</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -1565,15 +1616,38 @@
         <v>43627.451388888891</v>
       </c>
       <c r="D40" s="1">
+        <v>11000013</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G40" s="1">
+        <v>13954859886</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="2">
+        <v>43627.416666666664</v>
+      </c>
+      <c r="C41" s="2">
+        <v>43627.451388888891</v>
+      </c>
+      <c r="D41" s="1">
         <v>11000017</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G41" s="1">
         <v>13350453791</v>
       </c>
     </row>

</xml_diff>